<commit_message>
Fixed error in De Jong Heesen Removed psy studies published 2021 onwards
</commit_message>
<xml_diff>
--- a/columns_with_missing_values.xlsx
+++ b/columns_with_missing_values.xlsx
@@ -4982,7 +4982,7 @@
       <c r="AO37" s="2"/>
       <c r="AP37" s="2"/>
       <c r="AQ37" s="2" t="n">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="AR37" s="2"/>
       <c r="AS37" s="2"/>
@@ -5608,7 +5608,7 @@
       <c r="AO43" s="2"/>
       <c r="AP43" s="2"/>
       <c r="AQ43" s="2" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="AR43" s="2"/>
       <c r="AS43" s="2"/>
@@ -5691,7 +5691,7 @@
       <c r="AO44" s="2"/>
       <c r="AP44" s="2"/>
       <c r="AQ44" s="2" t="n">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="AR44" s="2"/>
       <c r="AS44" s="2"/>
@@ -5774,7 +5774,7 @@
       <c r="AO45" s="2"/>
       <c r="AP45" s="2"/>
       <c r="AQ45" s="2" t="n">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="AR45" s="2"/>
       <c r="AS45" s="2"/>
@@ -6763,7 +6763,7 @@
       <c r="AO54" s="2"/>
       <c r="AP54" s="2"/>
       <c r="AQ54" s="2" t="n">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="AR54" s="2"/>
       <c r="AS54" s="2"/>
@@ -6850,7 +6850,7 @@
       <c r="AO55" s="2"/>
       <c r="AP55" s="2"/>
       <c r="AQ55" s="2" t="n">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="AR55" s="2"/>
       <c r="AS55" s="2"/>
@@ -6965,7 +6965,7 @@
       <c r="AO56" s="3"/>
       <c r="AP56" s="3"/>
       <c r="AQ56" s="3" t="n">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="AR56" s="3" t="n">
         <v>30</v>

</xml_diff>

<commit_message>
Just triple checking that the script runs. All good!
</commit_message>
<xml_diff>
--- a/columns_with_missing_values.xlsx
+++ b/columns_with_missing_values.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="181">
   <si>
     <t xml:space="preserve">psy_or_med</t>
   </si>
@@ -555,15 +555,6 @@
   </si>
   <si>
     <t xml:space="preserve">school counseling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yu, 2002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eas</t>
   </si>
 </sst>
 </file>
@@ -6008,18 +5999,38 @@
       <c r="H46" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
-      <c r="N46" s="2"/>
-      <c r="O46" s="2"/>
+      <c r="I46" s="2" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="J46" s="2" t="n">
+        <v>7.3</v>
+      </c>
+      <c r="K46" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="L46" s="2" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="M46" s="2" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="N46" s="2" t="n">
+        <v>58</v>
+      </c>
+      <c r="O46" s="2" t="n">
+        <v>13.4</v>
+      </c>
       <c r="P46" s="2"/>
-      <c r="Q46" s="2"/>
-      <c r="R46" s="2"/>
+      <c r="Q46" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="R46" s="2" t="n">
+        <v>13.8</v>
+      </c>
       <c r="S46" s="2"/>
-      <c r="T46" s="2"/>
+      <c r="T46" s="2" t="n">
+        <v>58</v>
+      </c>
       <c r="U46" s="2"/>
       <c r="V46" s="2"/>
       <c r="W46" s="2"/>
@@ -6060,7 +6071,7 @@
       <c r="AZ46" s="2"/>
       <c r="BA46" s="2"/>
       <c r="BB46" s="2" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="BC46" s="2"/>
       <c r="BD46" s="2"/>
@@ -7174,216 +7185,94 @@
       <c r="BJ56" s="2"/>
     </row>
     <row r="57">
-      <c r="A57" s="2" t="n">
+      <c r="A57" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2" t="s">
+      <c r="D57" s="3"/>
+      <c r="E57" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F57" s="2" t="s">
+      <c r="F57" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="G57" s="2" t="s">
+      <c r="G57" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="H57" s="2" t="s">
+      <c r="H57" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="I57" s="2"/>
-      <c r="J57" s="2"/>
-      <c r="K57" s="2"/>
-      <c r="L57" s="2"/>
-      <c r="M57" s="2"/>
-      <c r="N57" s="2"/>
-      <c r="O57" s="2"/>
-      <c r="P57" s="2"/>
-      <c r="Q57" s="2" t="n">
+      <c r="I57" s="3"/>
+      <c r="J57" s="3"/>
+      <c r="K57" s="3"/>
+      <c r="L57" s="3"/>
+      <c r="M57" s="3"/>
+      <c r="N57" s="3"/>
+      <c r="O57" s="3"/>
+      <c r="P57" s="3"/>
+      <c r="Q57" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="R57" s="2"/>
-      <c r="S57" s="2"/>
-      <c r="T57" s="2" t="n">
+      <c r="R57" s="3"/>
+      <c r="S57" s="3"/>
+      <c r="T57" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="U57" s="2"/>
-      <c r="V57" s="2"/>
-      <c r="W57" s="2"/>
-      <c r="X57" s="2"/>
-      <c r="Y57" s="2"/>
-      <c r="Z57" s="2"/>
-      <c r="AA57" s="2"/>
-      <c r="AB57" s="2"/>
-      <c r="AC57" s="2"/>
-      <c r="AD57" s="2"/>
-      <c r="AE57" s="2"/>
-      <c r="AF57" s="2"/>
-      <c r="AG57" s="2"/>
-      <c r="AH57" s="2"/>
-      <c r="AI57" s="2"/>
-      <c r="AJ57" s="2"/>
-      <c r="AK57" s="2"/>
-      <c r="AL57" s="2"/>
-      <c r="AM57" s="2"/>
-      <c r="AN57" s="2"/>
-      <c r="AO57" s="2"/>
-      <c r="AP57" s="2"/>
-      <c r="AQ57" s="2"/>
-      <c r="AR57" s="2" t="n">
+      <c r="U57" s="3"/>
+      <c r="V57" s="3"/>
+      <c r="W57" s="3"/>
+      <c r="X57" s="3"/>
+      <c r="Y57" s="3"/>
+      <c r="Z57" s="3"/>
+      <c r="AA57" s="3"/>
+      <c r="AB57" s="3"/>
+      <c r="AC57" s="3"/>
+      <c r="AD57" s="3"/>
+      <c r="AE57" s="3"/>
+      <c r="AF57" s="3"/>
+      <c r="AG57" s="3"/>
+      <c r="AH57" s="3"/>
+      <c r="AI57" s="3"/>
+      <c r="AJ57" s="3"/>
+      <c r="AK57" s="3"/>
+      <c r="AL57" s="3"/>
+      <c r="AM57" s="3"/>
+      <c r="AN57" s="3"/>
+      <c r="AO57" s="3"/>
+      <c r="AP57" s="3"/>
+      <c r="AQ57" s="3"/>
+      <c r="AR57" s="3" t="n">
         <v>107</v>
       </c>
-      <c r="AS57" s="2"/>
-      <c r="AT57" s="2"/>
-      <c r="AU57" s="2"/>
-      <c r="AV57" s="2"/>
-      <c r="AW57" s="2" t="s">
+      <c r="AS57" s="3"/>
+      <c r="AT57" s="3"/>
+      <c r="AU57" s="3"/>
+      <c r="AV57" s="3"/>
+      <c r="AW57" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="AX57" s="2"/>
-      <c r="AY57" s="2" t="n">
+      <c r="AX57" s="3"/>
+      <c r="AY57" s="3" t="n">
         <v>14.54</v>
       </c>
-      <c r="AZ57" s="2"/>
-      <c r="BA57" s="2"/>
-      <c r="BB57" s="2" t="n">
+      <c r="AZ57" s="3"/>
+      <c r="BA57" s="3"/>
+      <c r="BB57" s="3" t="n">
         <v>59</v>
       </c>
-      <c r="BC57" s="2"/>
-      <c r="BD57" s="2"/>
-      <c r="BE57" s="2"/>
-      <c r="BF57" s="2"/>
-      <c r="BG57" s="2"/>
-      <c r="BH57" s="2"/>
-      <c r="BI57" s="2"/>
-      <c r="BJ57" s="2"/>
-    </row>
-    <row r="58">
-      <c r="A58" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="H58" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="I58" s="3" t="n">
-        <v>17.44</v>
-      </c>
-      <c r="J58" s="3"/>
-      <c r="K58" s="3" t="n">
-        <v>104</v>
-      </c>
-      <c r="L58" s="3" t="n">
-        <v>16.72</v>
-      </c>
-      <c r="M58" s="3"/>
-      <c r="N58" s="3" t="n">
-        <v>116</v>
-      </c>
-      <c r="O58" s="3" t="n">
-        <v>13.64</v>
-      </c>
-      <c r="P58" s="3" t="n">
-        <v>9.01</v>
-      </c>
-      <c r="Q58" s="3" t="n">
-        <v>101</v>
-      </c>
-      <c r="R58" s="3" t="n">
-        <v>16.02</v>
-      </c>
-      <c r="S58" s="3" t="n">
-        <v>10.16</v>
-      </c>
-      <c r="T58" s="3" t="n">
-        <v>114</v>
-      </c>
-      <c r="U58" s="3"/>
-      <c r="V58" s="3"/>
-      <c r="W58" s="3"/>
-      <c r="X58" s="3"/>
-      <c r="Y58" s="3"/>
-      <c r="Z58" s="3"/>
-      <c r="AA58" s="3"/>
-      <c r="AB58" s="3"/>
-      <c r="AC58" s="3"/>
-      <c r="AD58" s="3"/>
-      <c r="AE58" s="3"/>
-      <c r="AF58" s="3"/>
-      <c r="AG58" s="3"/>
-      <c r="AH58" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="AI58" s="3" t="n">
-        <v>34</v>
-      </c>
-      <c r="AJ58" s="3" t="n">
-        <v>0.288461538461538</v>
-      </c>
-      <c r="AK58" s="3" t="n">
-        <v>0.293103448275862</v>
-      </c>
-      <c r="AL58" s="3" t="n">
-        <v>0.297029702970297</v>
-      </c>
-      <c r="AM58" s="3" t="n">
-        <v>0.298245614035088</v>
-      </c>
-      <c r="AN58" s="3"/>
-      <c r="AO58" s="3"/>
-      <c r="AP58" s="3"/>
-      <c r="AQ58" s="3"/>
-      <c r="AR58" s="3" t="n">
-        <v>110</v>
-      </c>
-      <c r="AS58" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="AT58" s="3" t="n">
-        <v>26</v>
-      </c>
-      <c r="AU58" s="3"/>
-      <c r="AV58" s="3"/>
-      <c r="AW58" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="AX58" s="3"/>
-      <c r="AY58" s="3" t="n">
-        <v>11.8</v>
-      </c>
-      <c r="AZ58" s="3"/>
-      <c r="BA58" s="3"/>
-      <c r="BB58" s="3" t="n">
-        <v>45</v>
-      </c>
-      <c r="BC58" s="3"/>
-      <c r="BD58" s="3"/>
-      <c r="BE58" s="3"/>
-      <c r="BF58" s="3"/>
-      <c r="BG58" s="3"/>
-      <c r="BH58" s="3"/>
-      <c r="BI58" s="3"/>
-      <c r="BJ58" s="3"/>
+      <c r="BC57" s="3"/>
+      <c r="BD57" s="3"/>
+      <c r="BE57" s="3"/>
+      <c r="BF57" s="3"/>
+      <c r="BG57" s="3"/>
+      <c r="BH57" s="3"/>
+      <c r="BI57" s="3"/>
+      <c r="BJ57" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Debugging and fixing a few small errors
</commit_message>
<xml_diff>
--- a/columns_with_missing_values.xlsx
+++ b/columns_with_missing_values.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="187">
   <si>
     <t xml:space="preserve">psy_or_med</t>
   </si>
@@ -257,7 +257,7 @@
     <t xml:space="preserve">Atkinson</t>
   </si>
   <si>
-    <t xml:space="preserve">2014.0</t>
+    <t xml:space="preserve">2014</t>
   </si>
   <si>
     <t xml:space="preserve">Placebo</t>
@@ -278,7 +278,7 @@
     <t xml:space="preserve">Berard</t>
   </si>
   <si>
-    <t xml:space="preserve">2006.0</t>
+    <t xml:space="preserve">2006</t>
   </si>
   <si>
     <t xml:space="preserve">madrs</t>
@@ -332,7 +332,7 @@
     <t xml:space="preserve">Emslie</t>
   </si>
   <si>
-    <t xml:space="preserve">1997.0</t>
+    <t xml:space="preserve">1997</t>
   </si>
   <si>
     <t xml:space="preserve">Dysthymia, anxiety disordes, ADHD, oppositional/conduct disorder</t>
@@ -380,9 +380,6 @@
     <t xml:space="preserve">*Did not report demographics (e.g. mean age, % of women) per trial. Instead, demographics were reported for the two trials combined, hence the (combined)</t>
   </si>
   <si>
-    <t xml:space="preserve">2009.0</t>
-  </si>
-  <si>
     <t xml:space="preserve">40% improvement from baseline score</t>
   </si>
   <si>
@@ -410,7 +407,7 @@
     <t xml:space="preserve">Hughes</t>
   </si>
   <si>
-    <t xml:space="preserve">1990.0</t>
+    <t xml:space="preserve">1990</t>
   </si>
   <si>
     <t xml:space="preserve">50% reduction in CDRS</t>
@@ -425,7 +422,7 @@
     <t xml:space="preserve">Keller</t>
   </si>
   <si>
-    <t xml:space="preserve">2001.0</t>
+    <t xml:space="preserve">2001</t>
   </si>
   <si>
     <t xml:space="preserve">Anxiety disorders (e.g. separation anxiety, social anxiety disorder) and externalising disorders</t>
@@ -437,7 +434,7 @@
     <t xml:space="preserve">Klein</t>
   </si>
   <si>
-    <t xml:space="preserve">1998.0</t>
+    <t xml:space="preserve">1998</t>
   </si>
   <si>
     <t xml:space="preserve">Anxiety disorders and behaviour disorders</t>
@@ -449,7 +446,7 @@
     <t xml:space="preserve">Kutcher</t>
   </si>
   <si>
-    <t xml:space="preserve">1994.0</t>
+    <t xml:space="preserve">1994</t>
   </si>
   <si>
     <t xml:space="preserve">Canada</t>
@@ -482,9 +479,6 @@
     <t xml:space="preserve">March</t>
   </si>
   <si>
-    <t xml:space="preserve">2004.0</t>
-  </si>
-  <si>
     <t xml:space="preserve">Anxiety, disruptive behaviour, obsessive-compulsice/tic, substance use, attention-deficit/hyperactivity</t>
   </si>
   <si>
@@ -503,9 +497,6 @@
     <t xml:space="preserve">Sanford, 2006</t>
   </si>
   <si>
-    <t xml:space="preserve">2006</t>
-  </si>
-  <si>
     <t xml:space="preserve">Family Psychoeducation (FPE) + cau</t>
   </si>
   <si>
@@ -548,7 +539,7 @@
     <t xml:space="preserve">Wagner</t>
   </si>
   <si>
-    <t xml:space="preserve">2003.0</t>
+    <t xml:space="preserve">2003</t>
   </si>
   <si>
     <t xml:space="preserve">40% improvement</t>
@@ -3971,7 +3962,7 @@
         <v>105</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>122</v>
+        <v>69</v>
       </c>
       <c r="D25" s="2" t="n">
         <v>28</v>
@@ -4027,7 +4018,7 @@
         <v>157</v>
       </c>
       <c r="AA25" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AB25" s="2" t="n">
         <v>91</v>
@@ -4067,7 +4058,7 @@
         <v>8</v>
       </c>
       <c r="AW25" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AX25" s="2" t="s">
         <v>85</v>
@@ -4096,7 +4087,7 @@
         <v>58.6</v>
       </c>
       <c r="BH25" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BI25" s="2"/>
       <c r="BJ25" s="2" t="n">
@@ -4125,7 +4116,7 @@
         <v>105</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>122</v>
+        <v>69</v>
       </c>
       <c r="D26" s="2" t="n">
         <v>29</v>
@@ -4195,7 +4186,7 @@
         <v>8</v>
       </c>
       <c r="AW26" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AX26" s="2" t="s">
         <v>85</v>
@@ -4301,7 +4292,7 @@
         <v>117</v>
       </c>
       <c r="AA27" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AB27" s="2"/>
       <c r="AC27" s="2"/>
@@ -4334,7 +4325,7 @@
       </c>
       <c r="AW27" s="2"/>
       <c r="AX27" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AY27" s="2" t="s">
         <v>86</v>
@@ -4360,7 +4351,7 @@
         <v>56.6</v>
       </c>
       <c r="BH27" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="BI27" s="2"/>
       <c r="BJ27" s="2" t="n">
@@ -4449,7 +4440,7 @@
         <v>117</v>
       </c>
       <c r="AA28" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AB28" s="2"/>
       <c r="AC28" s="2"/>
@@ -4482,7 +4473,7 @@
       </c>
       <c r="AW28" s="2"/>
       <c r="AX28" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AY28" s="2" t="s">
         <v>86</v>
@@ -4595,7 +4586,7 @@
         <v>117</v>
       </c>
       <c r="AA29" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AB29" s="2"/>
       <c r="AC29" s="2"/>
@@ -4628,7 +4619,7 @@
       </c>
       <c r="AW29" s="2"/>
       <c r="AX29" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AY29" s="2" t="s">
         <v>86</v>
@@ -4678,10 +4669,10 @@
         <v>0</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>122</v>
+        <v>69</v>
       </c>
       <c r="D30" s="2" t="n">
         <v>35</v>
@@ -4751,7 +4742,7 @@
         <v>8</v>
       </c>
       <c r="AW30" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AX30" s="2" t="s">
         <v>85</v>
@@ -4802,10 +4793,10 @@
         <v>0</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="D31" s="2" t="n">
         <v>40</v>
@@ -4837,7 +4828,7 @@
       <c r="Y31" s="2"/>
       <c r="Z31" s="2"/>
       <c r="AA31" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AB31" s="2" t="n">
         <v>4</v>
@@ -4875,11 +4866,11 @@
         <v>6</v>
       </c>
       <c r="AW31" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AX31" s="2"/>
       <c r="AY31" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AZ31" s="2"/>
       <c r="BA31" s="2"/>
@@ -4904,10 +4895,10 @@
         <v>0</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="D32" s="2" t="n">
         <v>41</v>
@@ -4939,7 +4930,7 @@
       <c r="Y32" s="2"/>
       <c r="Z32" s="2"/>
       <c r="AA32" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AB32" s="2" t="n">
         <v>2</v>
@@ -4977,11 +4968,11 @@
         <v>6</v>
       </c>
       <c r="AW32" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AX32" s="2"/>
       <c r="AY32" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AZ32" s="2"/>
       <c r="BA32" s="2"/>
@@ -5006,10 +4997,10 @@
         <v>0</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="D33" s="2" t="n">
         <v>47</v>
@@ -5079,13 +5070,13 @@
         <v>8</v>
       </c>
       <c r="AW33" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AX33" s="2" t="s">
         <v>112</v>
       </c>
       <c r="AY33" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AZ33" s="2" t="n">
         <v>14.9</v>
@@ -5122,10 +5113,10 @@
         <v>0</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="D34" s="2" t="n">
         <v>44</v>
@@ -5195,13 +5186,13 @@
         <v>8</v>
       </c>
       <c r="AW34" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AX34" s="2" t="s">
         <v>112</v>
       </c>
       <c r="AY34" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AZ34" s="2" t="n">
         <v>14.8</v>
@@ -5238,10 +5229,10 @@
         <v>0</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="D35" s="2" t="n">
         <v>50</v>
@@ -5311,13 +5302,13 @@
         <v>6</v>
       </c>
       <c r="AW35" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AX35" s="2" t="s">
         <v>85</v>
       </c>
       <c r="AY35" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AZ35" s="2"/>
       <c r="BA35" s="2"/>
@@ -5354,10 +5345,10 @@
         <v>0</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="D36" s="2" t="n">
         <v>53</v>
@@ -5428,10 +5419,10 @@
       </c>
       <c r="AW36" s="2"/>
       <c r="AX36" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="AY36" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="AY36" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="AZ36" s="2"/>
       <c r="BA36" s="2"/>
@@ -5466,23 +5457,23 @@
         <v>1</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>149</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>70</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
@@ -5560,10 +5551,10 @@
         <v>1</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -5676,10 +5667,10 @@
         <v>1</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -5688,7 +5679,7 @@
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I39" s="2" t="n">
         <v>78.69</v>
@@ -5790,10 +5781,10 @@
         <v>0</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D40" s="2" t="n">
         <v>58</v>
@@ -5863,7 +5854,7 @@
         <v>12</v>
       </c>
       <c r="AW40" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="AX40" s="2" t="s">
         <v>85</v>
@@ -5906,7 +5897,7 @@
         <v>0</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>100</v>
@@ -6002,7 +5993,7 @@
         <v>56.8</v>
       </c>
       <c r="BH41" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="BI41" s="2"/>
       <c r="BJ41" s="2" t="n">
@@ -6024,7 +6015,7 @@
         <v>0</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>104</v>
@@ -6140,10 +6131,10 @@
         <v>0</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>122</v>
+        <v>69</v>
       </c>
       <c r="D43" s="2" t="n">
         <v>59</v>
@@ -6222,7 +6213,7 @@
       </c>
       <c r="AW43" s="2"/>
       <c r="AX43" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="AY43" s="2" t="s">
         <v>86</v>
@@ -6272,10 +6263,10 @@
         <v>0</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>122</v>
+        <v>69</v>
       </c>
       <c r="D44" s="2" t="n">
         <v>60</v>
@@ -6346,7 +6337,7 @@
       </c>
       <c r="AW44" s="2"/>
       <c r="AX44" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="AY44" s="2" t="s">
         <v>86</v>
@@ -6386,23 +6377,23 @@
         <v>1</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>70</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -6458,7 +6449,7 @@
       <c r="AV45" s="2"/>
       <c r="AW45" s="2"/>
       <c r="AX45" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="AY45" s="2"/>
       <c r="AZ45" s="2" t="n">
@@ -6500,23 +6491,23 @@
         <v>1</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>71</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="I46" s="2" t="n">
         <v>25.3</v>
@@ -6626,10 +6617,10 @@
         <v>1</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2" t="s">
@@ -6732,7 +6723,7 @@
         <v>0</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>88</v>
@@ -6814,10 +6805,10 @@
       </c>
       <c r="AW48" s="2"/>
       <c r="AX48" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="AY48" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AZ48" s="2" t="n">
         <v>16</v>
@@ -6840,7 +6831,7 @@
       <c r="BF48" s="2"/>
       <c r="BG48" s="2"/>
       <c r="BH48" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="BI48" s="2"/>
       <c r="BJ48" s="2"/>
@@ -6864,7 +6855,7 @@
         <v>0</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>88</v>
@@ -6915,7 +6906,7 @@
       <c r="Y49" s="2"/>
       <c r="Z49" s="2"/>
       <c r="AA49" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="AB49" s="2"/>
       <c r="AC49" s="2"/>
@@ -6946,10 +6937,10 @@
       </c>
       <c r="AW49" s="2"/>
       <c r="AX49" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="AY49" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AZ49" s="2" t="n">
         <v>16</v>
@@ -6994,10 +6985,10 @@
         <v>0</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D50" s="2" t="n">
         <v>64</v>
@@ -7049,7 +7040,7 @@
       <c r="Y50" s="2"/>
       <c r="Z50" s="2"/>
       <c r="AA50" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="AB50" s="2" t="n">
         <v>128</v>
@@ -7089,13 +7080,13 @@
         <v>10</v>
       </c>
       <c r="AW50" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AX50" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="AY50" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="AZ50" s="2"/>
       <c r="BA50" s="2"/>
@@ -7126,10 +7117,10 @@
         <v>0</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D51" s="2" t="n">
         <v>65</v>
@@ -7199,10 +7190,10 @@
         <v>10</v>
       </c>
       <c r="AW51" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AX51" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="AY51" s="2" t="s">
         <v>86</v>
@@ -7234,10 +7225,10 @@
         <v>0</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D52" s="2" t="n">
         <v>66</v>
@@ -7285,7 +7276,7 @@
       <c r="Y52" s="2"/>
       <c r="Z52" s="2"/>
       <c r="AA52" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="AB52" s="2" t="n">
         <v>32</v>
@@ -7325,7 +7316,7 @@
         <v>8</v>
       </c>
       <c r="AW52" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="AX52" s="2" t="s">
         <v>85</v>
@@ -7380,10 +7371,10 @@
         <v>0</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D53" s="2" t="n">
         <v>67</v>
@@ -7453,7 +7444,7 @@
         <v>8</v>
       </c>
       <c r="AW53" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="AX53" s="2" t="s">
         <v>85</v>
@@ -7500,7 +7491,7 @@
         <v>0</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>88</v>
@@ -7551,7 +7542,7 @@
         <v>132</v>
       </c>
       <c r="AA54" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="AB54" s="2" t="n">
         <v>59</v>
@@ -7591,13 +7582,13 @@
         <v>8</v>
       </c>
       <c r="AW54" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="AX54" s="2" t="s">
         <v>85</v>
       </c>
       <c r="AY54" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="AZ54" s="2" t="n">
         <v>12.2</v>
@@ -7648,7 +7639,7 @@
         <v>0</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>88</v>
@@ -7721,13 +7712,13 @@
         <v>8</v>
       </c>
       <c r="AW55" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="AX55" s="2" t="s">
         <v>85</v>
       </c>
       <c r="AY55" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="AZ55" s="2" t="n">
         <v>12.2</v>
@@ -7772,20 +7763,20 @@
         <v>1</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H56" s="2" t="s">
         <v>83</v>
@@ -7882,23 +7873,23 @@
         <v>1</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D57" s="3"/>
       <c r="E57" s="3" t="s">
         <v>70</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>

</xml_diff>

<commit_message>
Quite a few changes
</commit_message>
<xml_diff>
--- a/columns_with_missing_values.xlsx
+++ b/columns_with_missing_values.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="188">
   <si>
     <t xml:space="preserve">psy_or_med</t>
   </si>
@@ -191,6 +191,9 @@
     <t xml:space="preserve">control_percent_women</t>
   </si>
   <si>
+    <t xml:space="preserve">no_sites</t>
+  </si>
+  <si>
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
@@ -260,6 +263,9 @@
     <t xml:space="preserve">7 to 17</t>
   </si>
   <si>
+    <t xml:space="preserve">65</t>
+  </si>
+  <si>
     <t xml:space="preserve">Berard</t>
   </si>
   <si>
@@ -281,6 +287,9 @@
     <t xml:space="preserve">12 to 19</t>
   </si>
   <si>
+    <t xml:space="preserve">33</t>
+  </si>
+  <si>
     <t xml:space="preserve">bdi</t>
   </si>
   <si>
@@ -305,7 +314,7 @@
     <t xml:space="preserve">missing</t>
   </si>
   <si>
-    <t xml:space="preserve">FDA Trial - Poor reporting</t>
+    <t xml:space="preserve">15</t>
   </si>
   <si>
     <t xml:space="preserve">hamd</t>
@@ -323,6 +332,9 @@
     <t xml:space="preserve">Dysthymia, anxiety disordes, ADHD, oppositional/conduct disorder</t>
   </si>
   <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
     <t xml:space="preserve">ADHD, oppositional defiant disorder, conduct disorder</t>
   </si>
   <si>
@@ -338,7 +350,7 @@
     <t xml:space="preserve">USA + Canada</t>
   </si>
   <si>
-    <t xml:space="preserve">adhd was the most prevalent psychiatric condition, but others were not listed.</t>
+    <t xml:space="preserve">40</t>
   </si>
   <si>
     <t xml:space="preserve">2007 (combined)</t>
@@ -347,7 +359,7 @@
     <t xml:space="preserve">50% improvement from baseline score</t>
   </si>
   <si>
-    <t xml:space="preserve">*Did not report secondary outcome measures per trial. Instead they reported MADRS &amp; HAM-D scores for the combined population, hence why n is larger.</t>
+    <t xml:space="preserve">50</t>
   </si>
   <si>
     <t xml:space="preserve">2007a</t>
@@ -356,31 +368,22 @@
     <t xml:space="preserve">35% improvement from baseline score</t>
   </si>
   <si>
-    <t xml:space="preserve">*In this study, there were two trials (two groups of fluox, two groups of placebo). CDRS scores were reported per trial (fluox v placebo; fluox v placebo)</t>
-  </si>
-  <si>
     <t xml:space="preserve">2007b</t>
   </si>
   <si>
-    <t xml:space="preserve">*Did not report demographics (e.g. mean age, % of women) per trial. Instead, demographics were reported for the two trials combined, hence the (combined)</t>
-  </si>
-  <si>
     <t xml:space="preserve">40% improvement from baseline score</t>
   </si>
   <si>
     <t xml:space="preserve">ADHD, enuresis, GAD</t>
   </si>
   <si>
-    <t xml:space="preserve">Has two response criteria (40% improvement, and CGI-I)</t>
-  </si>
-  <si>
     <t xml:space="preserve">50% improvement from baseline scores</t>
   </si>
   <si>
     <t xml:space="preserve">USA, Mexico, Canada, Argentina</t>
   </si>
   <si>
-    <t xml:space="preserve">*Had four conditions (duloxetine 60mg, duloxetine 30mg, fluoxetine 20mg, placebo)</t>
+    <t xml:space="preserve">60</t>
   </si>
   <si>
     <t xml:space="preserve">Findling</t>
@@ -416,6 +419,9 @@
     <t xml:space="preserve">12 to 18</t>
   </si>
   <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
     <t xml:space="preserve">Klein</t>
   </si>
   <si>
@@ -467,10 +473,13 @@
     <t xml:space="preserve">Anxiety, disruptive behaviour, obsessive-compulsice/tic, substance use, attention-deficit/hyperactivity</t>
   </si>
   <si>
+    <t xml:space="preserve">13</t>
+  </si>
+  <si>
     <t xml:space="preserve">Organon</t>
   </si>
   <si>
-    <t xml:space="preserve">FDA trial - poor reporting</t>
+    <t xml:space="preserve">17</t>
   </si>
   <si>
     <t xml:space="preserve">Paxil (GlaxoSmithKline)</t>
@@ -515,7 +524,7 @@
     <t xml:space="preserve">European, multi-centered (31 recruitment sites)</t>
   </si>
   <si>
-    <t xml:space="preserve">*Ask Charlotte to check paper</t>
+    <t xml:space="preserve">31</t>
   </si>
   <si>
     <t xml:space="preserve">K-SADS depression and anhedonia scores ≤2</t>
@@ -539,13 +548,22 @@
     <t xml:space="preserve">6 to 17</t>
   </si>
   <si>
+    <t xml:space="preserve">53</t>
+  </si>
+  <si>
     <t xml:space="preserve">CDRS score ≤28</t>
   </si>
   <si>
     <t xml:space="preserve">Dysthmia, enuresis</t>
   </si>
   <si>
+    <t xml:space="preserve">21</t>
+  </si>
+  <si>
     <t xml:space="preserve">Anxiety disorders (e.g. GAD, panic disorder, social phobia, specific phobia)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25</t>
   </si>
   <si>
     <t xml:space="preserve">Young, 2010</t>
@@ -1117,26 +1135,29 @@
       <c r="BK1" t="s">
         <v>62</v>
       </c>
+      <c r="BL1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -1185,7 +1206,7 @@
       <c r="AV2" s="1"/>
       <c r="AW2" s="1"/>
       <c r="AX2" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AY2" s="1"/>
       <c r="AZ2" s="1"/>
@@ -1202,29 +1223,30 @@
       <c r="BI2" s="1"/>
       <c r="BJ2" s="1"/>
       <c r="BK2" s="1"/>
+      <c r="BL2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1284,7 +1306,7 @@
       <c r="AV3" s="2"/>
       <c r="AW3" s="2"/>
       <c r="AX3" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AY3" s="2"/>
       <c r="AZ3" s="2"/>
@@ -1299,27 +1321,28 @@
       <c r="BI3" s="2"/>
       <c r="BJ3" s="2"/>
       <c r="BK3" s="2"/>
+      <c r="BL3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>3</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I4" s="2" t="n">
         <v>59.2</v>
@@ -1360,7 +1383,7 @@
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
       <c r="AA4" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
@@ -1391,10 +1414,10 @@
       </c>
       <c r="AW4" s="2"/>
       <c r="AX4" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AY4" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AZ4" s="2" t="n">
         <v>13.1</v>
@@ -1416,31 +1439,34 @@
       <c r="BG4" s="2" t="n">
         <v>49.5</v>
       </c>
-      <c r="BH4" s="2"/>
+      <c r="BH4" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="BI4" s="2"/>
       <c r="BJ4" s="2"/>
       <c r="BK4" s="2"/>
+      <c r="BL4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I5" s="2" t="n">
         <v>58.8</v>
@@ -1481,7 +1507,7 @@
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
       <c r="AA5" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
@@ -1512,10 +1538,10 @@
       </c>
       <c r="AW5" s="2"/>
       <c r="AX5" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AY5" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AZ5" s="2" t="n">
         <v>13.1</v>
@@ -1537,31 +1563,34 @@
       <c r="BG5" s="2" t="n">
         <v>49.5</v>
       </c>
-      <c r="BH5" s="2"/>
+      <c r="BH5" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="BI5" s="2"/>
       <c r="BJ5" s="2"/>
       <c r="BK5" s="2"/>
+      <c r="BL5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>5</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I6" s="2" t="n">
         <v>25.9</v>
@@ -1610,7 +1639,7 @@
         <v>91</v>
       </c>
       <c r="AA6" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="AB6" s="2" t="n">
         <v>107</v>
@@ -1648,13 +1677,13 @@
         <v>12</v>
       </c>
       <c r="AW6" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="AX6" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="AY6" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="AZ6" s="2" t="n">
         <v>15.5</v>
@@ -1676,31 +1705,34 @@
       <c r="BG6" s="2" t="n">
         <v>67</v>
       </c>
-      <c r="BH6" s="2"/>
+      <c r="BH6" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="BI6" s="2"/>
       <c r="BJ6" s="2"/>
       <c r="BK6" s="2"/>
+      <c r="BL6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="I7" s="2" t="n">
         <v>23</v>
@@ -1749,7 +1781,7 @@
         <v>90</v>
       </c>
       <c r="AA7" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
@@ -1775,13 +1807,13 @@
         <v>12</v>
       </c>
       <c r="AW7" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="AX7" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="AY7" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="AZ7" s="2" t="n">
         <v>15.5</v>
@@ -1803,31 +1835,34 @@
       <c r="BG7" s="2" t="n">
         <v>67</v>
       </c>
-      <c r="BH7" s="2"/>
+      <c r="BH7" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="BI7" s="2"/>
       <c r="BJ7" s="2"/>
       <c r="BK7" s="2"/>
+      <c r="BL7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>6</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1892,13 +1927,13 @@
         <v>12</v>
       </c>
       <c r="AW8" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="AX8" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="AY8" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="AZ8" s="2" t="n">
         <v>15.5</v>
@@ -1920,31 +1955,34 @@
       <c r="BG8" s="2" t="n">
         <v>67</v>
       </c>
-      <c r="BH8" s="2"/>
+      <c r="BH8" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="BI8" s="2"/>
       <c r="BJ8" s="2"/>
       <c r="BK8" s="2"/>
+      <c r="BL8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>7</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1965,7 +2003,7 @@
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
       <c r="AA9" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AB9" s="2" t="n">
         <v>119</v>
@@ -2003,13 +2041,13 @@
         <v>12</v>
       </c>
       <c r="AW9" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="AX9" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="AY9" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="AZ9" s="2" t="n">
         <v>15.5</v>
@@ -2031,31 +2069,34 @@
       <c r="BG9" s="2" t="n">
         <v>67</v>
       </c>
-      <c r="BH9" s="2"/>
+      <c r="BH9" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="BI9" s="2"/>
       <c r="BJ9" s="2"/>
       <c r="BK9" s="2"/>
+      <c r="BL9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -2104,13 +2145,13 @@
         <v>8</v>
       </c>
       <c r="AW10" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="AX10" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AY10" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="AZ10" s="2"/>
       <c r="BA10" s="2"/>
@@ -2121,32 +2162,33 @@
       <c r="BF10" s="2"/>
       <c r="BG10" s="2"/>
       <c r="BH10" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="BI10" s="2"/>
       <c r="BJ10" s="2"/>
       <c r="BK10" s="2"/>
+      <c r="BL10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D11" s="2" t="n">
         <v>10</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -2195,13 +2237,13 @@
         <v>8</v>
       </c>
       <c r="AW11" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="AX11" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AY11" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="AZ11" s="2"/>
       <c r="BA11" s="2"/>
@@ -2211,31 +2253,34 @@
       <c r="BE11" s="2"/>
       <c r="BF11" s="2"/>
       <c r="BG11" s="2"/>
-      <c r="BH11" s="2"/>
+      <c r="BH11" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="BI11" s="2"/>
       <c r="BJ11" s="2"/>
       <c r="BK11" s="2"/>
+      <c r="BL11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D12" s="2" t="n">
         <v>11</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -2256,7 +2301,7 @@
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
       <c r="AA12" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
@@ -2286,13 +2331,13 @@
         <v>8</v>
       </c>
       <c r="AW12" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="AX12" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AY12" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="AZ12" s="2"/>
       <c r="BA12" s="2"/>
@@ -2302,31 +2347,34 @@
       <c r="BE12" s="2"/>
       <c r="BF12" s="2"/>
       <c r="BG12" s="2"/>
-      <c r="BH12" s="2"/>
+      <c r="BH12" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="BI12" s="2"/>
       <c r="BJ12" s="2"/>
       <c r="BK12" s="2"/>
+      <c r="BL12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D13" s="2" t="n">
         <v>12</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I13" s="2" t="n">
         <v>61.2</v>
@@ -2363,7 +2411,7 @@
         <v>93</v>
       </c>
       <c r="AA13" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
@@ -2389,13 +2437,13 @@
         <v>8</v>
       </c>
       <c r="AW13" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="AX13" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AY13" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="AZ13" s="2"/>
       <c r="BA13" s="2"/>
@@ -2405,31 +2453,34 @@
       <c r="BE13" s="2"/>
       <c r="BF13" s="2"/>
       <c r="BG13" s="2"/>
-      <c r="BH13" s="2"/>
+      <c r="BH13" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="BI13" s="2"/>
       <c r="BJ13" s="2"/>
       <c r="BK13" s="2"/>
+      <c r="BL13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D14" s="2" t="n">
         <v>15</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -2450,7 +2501,7 @@
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
       <c r="AA14" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AB14" s="2" t="n">
         <v>27</v>
@@ -2488,13 +2539,13 @@
         <v>8</v>
       </c>
       <c r="AW14" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="AX14" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AY14" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AZ14" s="2" t="n">
         <v>12.2</v>
@@ -2516,31 +2567,34 @@
       <c r="BG14" s="2" t="n">
         <v>46</v>
       </c>
-      <c r="BH14" s="2"/>
+      <c r="BH14" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="BI14" s="2"/>
       <c r="BJ14" s="2"/>
       <c r="BK14" s="2"/>
+      <c r="BL14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D15" s="2" t="n">
         <v>18</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -2561,7 +2615,7 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
       <c r="AA15" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AB15" s="2" t="n">
         <v>57</v>
@@ -2595,13 +2649,13 @@
         <v>9</v>
       </c>
       <c r="AW15" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="AX15" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AY15" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="AZ15" s="2" t="n">
         <v>12.7</v>
@@ -2623,31 +2677,34 @@
       <c r="BG15" s="2" t="n">
         <v>49.5</v>
       </c>
-      <c r="BH15" s="2"/>
+      <c r="BH15" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="BI15" s="2"/>
       <c r="BJ15" s="2"/>
       <c r="BK15" s="2"/>
+      <c r="BL15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D16" s="2" t="n">
         <v>19</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -2709,10 +2766,10 @@
       </c>
       <c r="AW16" s="2"/>
       <c r="AX16" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AY16" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="AZ16" s="2"/>
       <c r="BA16" s="2"/>
@@ -2722,31 +2779,34 @@
       <c r="BE16" s="2"/>
       <c r="BF16" s="2"/>
       <c r="BG16" s="2"/>
-      <c r="BH16" s="2"/>
+      <c r="BH16" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="BI16" s="2"/>
       <c r="BJ16" s="2"/>
       <c r="BK16" s="2"/>
+      <c r="BL16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D17" s="2" t="n">
         <v>20</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -2800,10 +2860,10 @@
       </c>
       <c r="AW17" s="2"/>
       <c r="AX17" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AY17" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="AZ17" s="2"/>
       <c r="BA17" s="2"/>
@@ -2813,31 +2873,34 @@
       <c r="BE17" s="2"/>
       <c r="BF17" s="2"/>
       <c r="BG17" s="2"/>
-      <c r="BH17" s="2"/>
+      <c r="BH17" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="BI17" s="2"/>
       <c r="BJ17" s="2"/>
       <c r="BK17" s="2"/>
+      <c r="BL17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D18" s="2" t="n">
         <v>21</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -2858,7 +2921,7 @@
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
       <c r="AA18" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AB18" s="2" t="n">
         <v>61</v>
@@ -2897,10 +2960,10 @@
       </c>
       <c r="AW18" s="2"/>
       <c r="AX18" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AY18" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="AZ18" s="2"/>
       <c r="BA18" s="2"/>
@@ -2910,31 +2973,34 @@
       <c r="BE18" s="2"/>
       <c r="BF18" s="2"/>
       <c r="BG18" s="2"/>
-      <c r="BH18" s="2"/>
+      <c r="BH18" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="BI18" s="2"/>
       <c r="BJ18" s="2"/>
       <c r="BK18" s="2"/>
+      <c r="BL18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D19" s="2" t="n">
         <v>22</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I19" s="2" t="n">
         <v>60.7</v>
@@ -3007,13 +3073,13 @@
         <v>8</v>
       </c>
       <c r="AW19" s="2" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="AX19" s="2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="AY19" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AZ19" s="2" t="n">
         <v>11.9</v>
@@ -3040,32 +3106,33 @@
         <v>46.8</v>
       </c>
       <c r="BH19" s="2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="BI19" s="2"/>
       <c r="BJ19" s="2"/>
       <c r="BK19" s="2"/>
+      <c r="BL19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D20" s="2" t="n">
         <v>23</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -3086,7 +3153,7 @@
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
       <c r="AA20" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AB20" s="2" t="n">
         <v>49</v>
@@ -3124,13 +3191,13 @@
         <v>8</v>
       </c>
       <c r="AW20" s="2" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="AX20" s="2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="AY20" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AZ20" s="2" t="n">
         <v>11.9</v>
@@ -3156,31 +3223,34 @@
       <c r="BG20" s="2" t="n">
         <v>46.8</v>
       </c>
-      <c r="BH20" s="2"/>
+      <c r="BH20" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="BI20" s="2"/>
       <c r="BJ20" s="2"/>
       <c r="BK20" s="2"/>
+      <c r="BL20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D21" s="2" t="n">
         <v>27</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="I21" s="2" t="n">
         <v>18.2</v>
@@ -3217,7 +3287,7 @@
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
       <c r="AA21" s="2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="AB21" s="2" t="n">
         <v>85</v>
@@ -3256,10 +3326,10 @@
       </c>
       <c r="AW21" s="2"/>
       <c r="AX21" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AY21" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AZ21" s="2" t="n">
         <v>12.2</v>
@@ -3281,31 +3351,34 @@
       <c r="BG21" s="2" t="n">
         <v>47</v>
       </c>
-      <c r="BH21" s="2"/>
+      <c r="BH21" s="2" t="s">
+        <v>115</v>
+      </c>
       <c r="BI21" s="2"/>
       <c r="BJ21" s="2"/>
       <c r="BK21" s="2"/>
+      <c r="BL21" s="2"/>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D22" s="2" t="n">
         <v>26</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I22" s="2" t="n">
         <v>25.6</v>
@@ -3342,7 +3415,7 @@
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
       <c r="AA22" s="2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="AB22" s="2" t="n">
         <v>81</v>
@@ -3381,10 +3454,10 @@
       </c>
       <c r="AW22" s="2"/>
       <c r="AX22" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AY22" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AZ22" s="2" t="n">
         <v>12.2</v>
@@ -3407,32 +3480,33 @@
         <v>47</v>
       </c>
       <c r="BH22" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="BI22" s="2"/>
       <c r="BJ22" s="2"/>
       <c r="BK22" s="2"/>
+      <c r="BL22" s="2"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D23" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I23" s="2" t="n">
         <v>54.4</v>
@@ -3473,7 +3547,7 @@
       <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
       <c r="AA23" s="2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="AB23" s="2" t="n">
         <v>43</v>
@@ -3532,10 +3606,10 @@
       </c>
       <c r="AW23" s="2"/>
       <c r="AX23" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AY23" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AZ23" s="2"/>
       <c r="BA23" s="2" t="n">
@@ -3550,32 +3624,33 @@
       <c r="BF23" s="2"/>
       <c r="BG23" s="2"/>
       <c r="BH23" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="BI23" s="2"/>
       <c r="BJ23" s="2"/>
       <c r="BK23" s="2"/>
+      <c r="BL23" s="2"/>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D24" s="2" t="n">
         <v>25</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I24" s="2" t="n">
         <v>57.3</v>
@@ -3616,7 +3691,7 @@
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
       <c r="AA24" s="2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="AB24" s="2" t="n">
         <v>77</v>
@@ -3675,10 +3750,10 @@
       </c>
       <c r="AW24" s="2"/>
       <c r="AX24" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AY24" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AZ24" s="2"/>
       <c r="BA24" s="2" t="n">
@@ -3693,32 +3768,33 @@
       <c r="BF24" s="2"/>
       <c r="BG24" s="2"/>
       <c r="BH24" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BI24" s="2"/>
       <c r="BJ24" s="2"/>
       <c r="BK24" s="2"/>
+      <c r="BL24" s="2"/>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D25" s="2" t="n">
         <v>28</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I25" s="2" t="n">
         <v>57.6</v>
@@ -3763,7 +3839,7 @@
         <v>157</v>
       </c>
       <c r="AA25" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="AB25" s="2" t="n">
         <v>91</v>
@@ -3801,13 +3877,13 @@
         <v>8</v>
       </c>
       <c r="AW25" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="AX25" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AY25" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="AZ25" s="2" t="n">
         <v>14.7</v>
@@ -3830,32 +3906,33 @@
         <v>58.6</v>
       </c>
       <c r="BH25" s="2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="BI25" s="2"/>
       <c r="BJ25" s="2"/>
       <c r="BK25" s="2"/>
+      <c r="BL25" s="2"/>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D26" s="2" t="n">
         <v>29</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -3876,7 +3953,7 @@
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
       <c r="AA26" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AB26" s="2" t="n">
         <v>99</v>
@@ -3914,13 +3991,13 @@
         <v>8</v>
       </c>
       <c r="AW26" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="AX26" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AY26" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="AZ26" s="2" t="n">
         <v>14.7</v>
@@ -3942,31 +4019,34 @@
       <c r="BG26" s="2" t="n">
         <v>58.6</v>
       </c>
-      <c r="BH26" s="2"/>
+      <c r="BH26" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="BI26" s="2"/>
       <c r="BJ26" s="2"/>
       <c r="BK26" s="2"/>
+      <c r="BL26" s="2"/>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D27" s="2" t="n">
         <v>30</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I27" s="2" t="n">
         <v>59.3</v>
@@ -4015,7 +4095,7 @@
         <v>117</v>
       </c>
       <c r="AA27" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AB27" s="2"/>
       <c r="AC27" s="2"/>
@@ -4046,10 +4126,10 @@
       </c>
       <c r="AW27" s="2"/>
       <c r="AX27" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AY27" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AZ27" s="2" t="n">
         <v>12.9</v>
@@ -4072,32 +4152,33 @@
         <v>56.6</v>
       </c>
       <c r="BH27" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="BI27" s="2"/>
       <c r="BJ27" s="2"/>
       <c r="BK27" s="2"/>
+      <c r="BL27" s="2"/>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D28" s="2" t="n">
         <v>31</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I28" s="2" t="n">
         <v>59.8</v>
@@ -4146,7 +4227,7 @@
         <v>117</v>
       </c>
       <c r="AA28" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AB28" s="2"/>
       <c r="AC28" s="2"/>
@@ -4177,10 +4258,10 @@
       </c>
       <c r="AW28" s="2"/>
       <c r="AX28" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AY28" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AZ28" s="2" t="n">
         <v>12.9</v>
@@ -4202,31 +4283,34 @@
       <c r="BG28" s="2" t="n">
         <v>56.6</v>
       </c>
-      <c r="BH28" s="2"/>
+      <c r="BH28" s="2" t="s">
+        <v>123</v>
+      </c>
       <c r="BI28" s="2"/>
       <c r="BJ28" s="2"/>
       <c r="BK28" s="2"/>
+      <c r="BL28" s="2"/>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D29" s="2" t="n">
         <v>32</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I29" s="2" t="n">
         <v>57.9</v>
@@ -4275,7 +4359,7 @@
         <v>117</v>
       </c>
       <c r="AA29" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AB29" s="2"/>
       <c r="AC29" s="2"/>
@@ -4306,10 +4390,10 @@
       </c>
       <c r="AW29" s="2"/>
       <c r="AX29" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AY29" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AZ29" s="2" t="n">
         <v>13</v>
@@ -4331,31 +4415,34 @@
       <c r="BG29" s="2" t="n">
         <v>56.6</v>
       </c>
-      <c r="BH29" s="2"/>
+      <c r="BH29" s="2" t="s">
+        <v>123</v>
+      </c>
       <c r="BI29" s="2"/>
       <c r="BJ29" s="2"/>
       <c r="BK29" s="2"/>
+      <c r="BL29" s="2"/>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D30" s="2" t="n">
         <v>35</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -4376,7 +4463,7 @@
       <c r="Y30" s="2"/>
       <c r="Z30" s="2"/>
       <c r="AA30" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AB30" s="2" t="n">
         <v>9</v>
@@ -4414,13 +4501,13 @@
         <v>8</v>
       </c>
       <c r="AW30" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AX30" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AY30" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="AZ30" s="2" t="n">
         <v>16.55</v>
@@ -4446,31 +4533,34 @@
       <c r="BG30" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="BH30" s="2"/>
+      <c r="BH30" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="BI30" s="2"/>
       <c r="BJ30" s="2"/>
       <c r="BK30" s="2"/>
+      <c r="BL30" s="2"/>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D31" s="2" t="n">
         <v>40</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
@@ -4491,7 +4581,7 @@
       <c r="Y31" s="2"/>
       <c r="Z31" s="2"/>
       <c r="AA31" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AB31" s="2" t="n">
         <v>4</v>
@@ -4529,11 +4619,11 @@
         <v>6</v>
       </c>
       <c r="AW31" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AX31" s="2"/>
       <c r="AY31" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AZ31" s="2"/>
       <c r="BA31" s="2"/>
@@ -4543,31 +4633,34 @@
       <c r="BE31" s="2"/>
       <c r="BF31" s="2"/>
       <c r="BG31" s="2"/>
-      <c r="BH31" s="2"/>
+      <c r="BH31" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="BI31" s="2"/>
       <c r="BJ31" s="2"/>
       <c r="BK31" s="2"/>
+      <c r="BL31" s="2"/>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D32" s="2" t="n">
         <v>41</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
@@ -4588,7 +4681,7 @@
       <c r="Y32" s="2"/>
       <c r="Z32" s="2"/>
       <c r="AA32" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AB32" s="2" t="n">
         <v>2</v>
@@ -4626,11 +4719,11 @@
         <v>6</v>
       </c>
       <c r="AW32" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AX32" s="2"/>
       <c r="AY32" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AZ32" s="2"/>
       <c r="BA32" s="2"/>
@@ -4640,31 +4733,34 @@
       <c r="BE32" s="2"/>
       <c r="BF32" s="2"/>
       <c r="BG32" s="2"/>
-      <c r="BH32" s="2"/>
+      <c r="BH32" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="BI32" s="2"/>
       <c r="BJ32" s="2"/>
       <c r="BK32" s="2"/>
+      <c r="BL32" s="2"/>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D33" s="2" t="n">
         <v>47</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
@@ -4685,7 +4781,7 @@
       <c r="Y33" s="2"/>
       <c r="Z33" s="2"/>
       <c r="AA33" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AB33" s="2" t="n">
         <v>49</v>
@@ -4723,13 +4819,13 @@
         <v>8</v>
       </c>
       <c r="AW33" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AX33" s="2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="AY33" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AZ33" s="2" t="n">
         <v>14.9</v>
@@ -4751,31 +4847,34 @@
       <c r="BG33" s="2" t="n">
         <v>65.5</v>
       </c>
-      <c r="BH33" s="2"/>
+      <c r="BH33" s="2" t="s">
+        <v>135</v>
+      </c>
       <c r="BI33" s="2"/>
       <c r="BJ33" s="2"/>
       <c r="BK33" s="2"/>
+      <c r="BL33" s="2"/>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D34" s="2" t="n">
         <v>44</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
@@ -4796,7 +4895,7 @@
       <c r="Y34" s="2"/>
       <c r="Z34" s="2"/>
       <c r="AA34" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AB34" s="2" t="n">
         <v>59</v>
@@ -4834,13 +4933,13 @@
         <v>8</v>
       </c>
       <c r="AW34" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AX34" s="2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="AY34" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AZ34" s="2" t="n">
         <v>14.8</v>
@@ -4862,31 +4961,34 @@
       <c r="BG34" s="2" t="n">
         <v>65.5</v>
       </c>
-      <c r="BH34" s="2"/>
+      <c r="BH34" s="2" t="s">
+        <v>135</v>
+      </c>
       <c r="BI34" s="2"/>
       <c r="BJ34" s="2"/>
       <c r="BK34" s="2"/>
+      <c r="BL34" s="2"/>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D35" s="2" t="n">
         <v>50</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
@@ -4907,7 +5009,7 @@
       <c r="Y35" s="2"/>
       <c r="Z35" s="2"/>
       <c r="AA35" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AB35" s="2" t="n">
         <v>12</v>
@@ -4945,13 +5047,13 @@
         <v>6</v>
       </c>
       <c r="AW35" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AX35" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AY35" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AZ35" s="2"/>
       <c r="BA35" s="2"/>
@@ -4969,31 +5071,34 @@
       <c r="BG35" s="2" t="n">
         <v>67</v>
       </c>
-      <c r="BH35" s="2"/>
+      <c r="BH35" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="BI35" s="2"/>
       <c r="BJ35" s="2"/>
       <c r="BK35" s="2"/>
+      <c r="BL35" s="2"/>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D36" s="2" t="n">
         <v>53</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
@@ -5051,10 +5156,10 @@
       </c>
       <c r="AW36" s="2"/>
       <c r="AX36" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="AY36" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="AZ36" s="2"/>
       <c r="BA36" s="2"/>
@@ -5070,33 +5175,36 @@
       <c r="BG36" s="2" t="n">
         <v>70</v>
       </c>
-      <c r="BH36" s="2"/>
+      <c r="BH36" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="BI36" s="2"/>
       <c r="BJ36" s="2"/>
       <c r="BK36" s="2"/>
+      <c r="BL36" s="2"/>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
@@ -5144,7 +5252,7 @@
       <c r="AV37" s="2"/>
       <c r="AW37" s="2"/>
       <c r="AX37" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AY37" s="2"/>
       <c r="AZ37" s="2"/>
@@ -5161,25 +5269,26 @@
       <c r="BI37" s="2"/>
       <c r="BJ37" s="2"/>
       <c r="BK37" s="2"/>
+      <c r="BL37" s="2"/>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I38" s="2" t="n">
         <v>59.64</v>
@@ -5247,7 +5356,7 @@
       <c r="AV38" s="2"/>
       <c r="AW38" s="2"/>
       <c r="AX38" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AY38" s="2"/>
       <c r="AZ38" s="2"/>
@@ -5264,29 +5373,30 @@
       <c r="BG38" s="2"/>
       <c r="BH38" s="2"/>
       <c r="BI38" s="2"/>
-      <c r="BJ38" s="2" t="n">
+      <c r="BJ38" s="2"/>
+      <c r="BK38" s="2" t="n">
         <v>-2.56642335766423</v>
       </c>
-      <c r="BK38" s="2"/>
+      <c r="BL38" s="2"/>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="I39" s="2" t="n">
         <v>78.69</v>
@@ -5352,7 +5462,7 @@
       <c r="AV39" s="2"/>
       <c r="AW39" s="2"/>
       <c r="AX39" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AY39" s="2"/>
       <c r="AZ39" s="2"/>
@@ -5369,31 +5479,32 @@
       <c r="BG39" s="2"/>
       <c r="BH39" s="2"/>
       <c r="BI39" s="2"/>
-      <c r="BJ39" s="2" t="n">
+      <c r="BJ39" s="2"/>
+      <c r="BK39" s="2" t="n">
         <v>-0.866370609608398</v>
       </c>
-      <c r="BK39" s="2"/>
+      <c r="BL39" s="2"/>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="D40" s="2" t="n">
         <v>58</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
@@ -5414,7 +5525,7 @@
       <c r="Y40" s="2"/>
       <c r="Z40" s="2"/>
       <c r="AA40" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AB40" s="2" t="n">
         <v>66</v>
@@ -5452,13 +5563,13 @@
         <v>12</v>
       </c>
       <c r="AW40" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AX40" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AY40" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="AZ40" s="2"/>
       <c r="BA40" s="2"/>
@@ -5476,31 +5587,34 @@
       <c r="BG40" s="2" t="n">
         <v>54.4</v>
       </c>
-      <c r="BH40" s="2"/>
+      <c r="BH40" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="BI40" s="2"/>
       <c r="BJ40" s="2"/>
       <c r="BK40" s="2"/>
+      <c r="BL40" s="2"/>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D41" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
@@ -5533,7 +5647,7 @@
       <c r="Y41" s="2"/>
       <c r="Z41" s="2"/>
       <c r="AA41" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="AB41" s="2"/>
       <c r="AC41" s="2"/>
@@ -5561,7 +5675,7 @@
       <c r="AW41" s="2"/>
       <c r="AX41" s="2"/>
       <c r="AY41" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AZ41" s="2" t="n">
         <v>12.3</v>
@@ -5580,37 +5694,38 @@
         <v>56.8</v>
       </c>
       <c r="BH41" s="2" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="BI41" s="2"/>
       <c r="BJ41" s="2"/>
       <c r="BK41" s="2"/>
+      <c r="BL41" s="2"/>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D42" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2" t="n">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
@@ -5638,7 +5753,7 @@
       <c r="Y42" s="2"/>
       <c r="Z42" s="2"/>
       <c r="AA42" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="AB42" s="2"/>
       <c r="AC42" s="2"/>
@@ -5666,7 +5781,7 @@
       <c r="AW42" s="2"/>
       <c r="AX42" s="2"/>
       <c r="AY42" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AZ42" s="2" t="n">
         <v>11.9</v>
@@ -5684,31 +5799,34 @@
       <c r="BG42" s="2" t="n">
         <v>50.5</v>
       </c>
-      <c r="BH42" s="2"/>
+      <c r="BH42" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="BI42" s="2"/>
       <c r="BJ42" s="2"/>
       <c r="BK42" s="2"/>
+      <c r="BL42" s="2"/>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D43" s="2" t="n">
         <v>59</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
@@ -5774,10 +5892,10 @@
       </c>
       <c r="AW43" s="2"/>
       <c r="AX43" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="AY43" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AZ43" s="2" t="n">
         <v>14.4</v>
@@ -5799,31 +5917,34 @@
       <c r="BG43" s="2" t="n">
         <v>66.7</v>
       </c>
-      <c r="BH43" s="2"/>
+      <c r="BH43" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="BI43" s="2"/>
       <c r="BJ43" s="2"/>
       <c r="BK43" s="2"/>
+      <c r="BL43" s="2"/>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D44" s="2" t="n">
         <v>60</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
@@ -5844,7 +5965,7 @@
       <c r="Y44" s="2"/>
       <c r="Z44" s="2"/>
       <c r="AA44" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AB44" s="2" t="n">
         <v>15</v>
@@ -5883,10 +6004,10 @@
       </c>
       <c r="AW44" s="2"/>
       <c r="AX44" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="AY44" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AZ44" s="2" t="n">
         <v>14.4</v>
@@ -5908,33 +6029,36 @@
       <c r="BG44" s="2" t="n">
         <v>66.7</v>
       </c>
-      <c r="BH44" s="2"/>
+      <c r="BH44" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="BI44" s="2"/>
       <c r="BJ44" s="2"/>
       <c r="BK44" s="2"/>
+      <c r="BL44" s="2"/>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -5990,7 +6114,7 @@
       <c r="AV45" s="2"/>
       <c r="AW45" s="2"/>
       <c r="AX45" s="2" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="AY45" s="2"/>
       <c r="AZ45" s="2" t="n">
@@ -6013,29 +6137,30 @@
       <c r="BI45" s="2"/>
       <c r="BJ45" s="2"/>
       <c r="BK45" s="2"/>
+      <c r="BL45" s="2"/>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="I46" s="2" t="n">
         <v>25.3</v>
@@ -6103,7 +6228,7 @@
       <c r="AV46" s="2"/>
       <c r="AW46" s="2"/>
       <c r="AX46" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AY46" s="2"/>
       <c r="AZ46" s="2" t="n">
@@ -6126,29 +6251,30 @@
       <c r="BI46" s="2"/>
       <c r="BJ46" s="2"/>
       <c r="BK46" s="2"/>
+      <c r="BL46" s="2"/>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F47" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G47" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G47" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="H47" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
@@ -6196,7 +6322,7 @@
       <c r="AV47" s="2"/>
       <c r="AW47" s="2"/>
       <c r="AX47" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AY47" s="2"/>
       <c r="AZ47" s="2" t="n">
@@ -6223,27 +6349,28 @@
       <c r="BI47" s="2"/>
       <c r="BJ47" s="2"/>
       <c r="BK47" s="2"/>
+      <c r="BL47" s="2"/>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D48" s="2" t="n">
         <v>63</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I48" s="2" t="n">
         <v>30</v>
@@ -6280,7 +6407,7 @@
       <c r="Y48" s="2"/>
       <c r="Z48" s="2"/>
       <c r="AA48" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="AB48" s="2"/>
       <c r="AC48" s="2"/>
@@ -6311,10 +6438,10 @@
       </c>
       <c r="AW48" s="2"/>
       <c r="AX48" s="2" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="AY48" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AZ48" s="2" t="n">
         <v>16</v>
@@ -6337,32 +6464,33 @@
       <c r="BF48" s="2"/>
       <c r="BG48" s="2"/>
       <c r="BH48" s="2" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="BI48" s="2"/>
       <c r="BJ48" s="2"/>
       <c r="BK48" s="2"/>
+      <c r="BL48" s="2"/>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D49" s="2" t="n">
         <v>62</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="I49" s="2" t="n">
         <v>32</v>
@@ -6399,7 +6527,7 @@
       <c r="Y49" s="2"/>
       <c r="Z49" s="2"/>
       <c r="AA49" s="2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="AB49" s="2"/>
       <c r="AC49" s="2"/>
@@ -6430,10 +6558,10 @@
       </c>
       <c r="AW49" s="2"/>
       <c r="AX49" s="2" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="AY49" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AZ49" s="2" t="n">
         <v>16</v>
@@ -6455,31 +6583,34 @@
       </c>
       <c r="BF49" s="2"/>
       <c r="BG49" s="2"/>
-      <c r="BH49" s="2"/>
+      <c r="BH49" s="2" t="s">
+        <v>170</v>
+      </c>
       <c r="BI49" s="2"/>
       <c r="BJ49" s="2"/>
       <c r="BK49" s="2"/>
+      <c r="BL49" s="2"/>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D50" s="2" t="n">
         <v>64</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I50" s="2" t="n">
         <v>64.3</v>
@@ -6520,7 +6651,7 @@
       <c r="Y50" s="2"/>
       <c r="Z50" s="2"/>
       <c r="AA50" s="2" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="AB50" s="2" t="n">
         <v>128</v>
@@ -6558,13 +6689,13 @@
         <v>10</v>
       </c>
       <c r="AW50" s="2" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="AX50" s="2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="AY50" s="2" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AZ50" s="2"/>
       <c r="BA50" s="2"/>
@@ -6578,31 +6709,34 @@
       <c r="BG50" s="2" t="n">
         <v>44.9</v>
       </c>
-      <c r="BH50" s="2"/>
+      <c r="BH50" s="2" t="s">
+        <v>178</v>
+      </c>
       <c r="BI50" s="2"/>
       <c r="BJ50" s="2"/>
       <c r="BK50" s="2"/>
+      <c r="BL50" s="2"/>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D51" s="2" t="n">
         <v>65</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
@@ -6623,7 +6757,7 @@
       <c r="Y51" s="2"/>
       <c r="Z51" s="2"/>
       <c r="AA51" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AB51" s="2" t="n">
         <v>117</v>
@@ -6661,13 +6795,13 @@
         <v>10</v>
       </c>
       <c r="AW51" s="2" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="AX51" s="2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="AY51" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AZ51" s="2"/>
       <c r="BA51" s="2"/>
@@ -6681,31 +6815,34 @@
       <c r="BG51" s="2" t="n">
         <v>44.9</v>
       </c>
-      <c r="BH51" s="2"/>
+      <c r="BH51" s="2" t="s">
+        <v>178</v>
+      </c>
       <c r="BI51" s="2"/>
       <c r="BJ51" s="2"/>
       <c r="BK51" s="2"/>
+      <c r="BL51" s="2"/>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D52" s="2" t="n">
         <v>66</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I52" s="2" t="n">
         <v>58.8</v>
@@ -6742,7 +6879,7 @@
       <c r="Y52" s="2"/>
       <c r="Z52" s="2"/>
       <c r="AA52" s="2" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="AB52" s="2" t="n">
         <v>32</v>
@@ -6780,13 +6917,13 @@
         <v>8</v>
       </c>
       <c r="AW52" s="2" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="AX52" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AY52" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AZ52" s="2" t="n">
         <v>12.1</v>
@@ -6810,31 +6947,34 @@
       <c r="BG52" s="2" t="n">
         <v>54.1</v>
       </c>
-      <c r="BH52" s="2"/>
+      <c r="BH52" s="2" t="s">
+        <v>181</v>
+      </c>
       <c r="BI52" s="2"/>
       <c r="BJ52" s="2"/>
       <c r="BK52" s="2"/>
+      <c r="BL52" s="2"/>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D53" s="2" t="n">
         <v>67</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
@@ -6855,7 +6995,7 @@
       <c r="Y53" s="2"/>
       <c r="Z53" s="2"/>
       <c r="AA53" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AB53" s="2" t="n">
         <v>42</v>
@@ -6893,13 +7033,13 @@
         <v>8</v>
       </c>
       <c r="AW53" s="2" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="AX53" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AY53" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AZ53" s="2" t="n">
         <v>12.1</v>
@@ -6923,31 +7063,34 @@
       <c r="BG53" s="2" t="n">
         <v>54.1</v>
       </c>
-      <c r="BH53" s="2"/>
+      <c r="BH53" s="2" t="s">
+        <v>181</v>
+      </c>
       <c r="BI53" s="2"/>
       <c r="BJ53" s="2"/>
       <c r="BK53" s="2"/>
+      <c r="BL53" s="2"/>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D54" s="2" t="n">
         <v>68</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I54" s="2" t="n">
         <v>54.5</v>
@@ -6984,7 +7127,7 @@
         <v>132</v>
       </c>
       <c r="AA54" s="2" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="AB54" s="2" t="n">
         <v>59</v>
@@ -7022,13 +7165,13 @@
         <v>8</v>
       </c>
       <c r="AW54" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="AX54" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AY54" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="AX54" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="AY54" s="2" t="s">
-        <v>174</v>
       </c>
       <c r="AZ54" s="2" t="n">
         <v>12.2</v>
@@ -7054,31 +7197,34 @@
       <c r="BG54" s="2" t="n">
         <v>51.9</v>
       </c>
-      <c r="BH54" s="2"/>
+      <c r="BH54" s="2" t="s">
+        <v>183</v>
+      </c>
       <c r="BI54" s="2"/>
       <c r="BJ54" s="2"/>
       <c r="BK54" s="2"/>
+      <c r="BL54" s="2"/>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D55" s="2" t="n">
         <v>69</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
@@ -7099,7 +7245,7 @@
       <c r="Y55" s="2"/>
       <c r="Z55" s="2"/>
       <c r="AA55" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AB55" s="2" t="n">
         <v>81</v>
@@ -7137,13 +7283,13 @@
         <v>8</v>
       </c>
       <c r="AW55" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="AX55" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AY55" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="AX55" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="AY55" s="2" t="s">
-        <v>174</v>
       </c>
       <c r="AZ55" s="2" t="n">
         <v>12.2</v>
@@ -7169,33 +7315,36 @@
       <c r="BG55" s="2" t="n">
         <v>51.9</v>
       </c>
-      <c r="BH55" s="2"/>
+      <c r="BH55" s="2" t="s">
+        <v>183</v>
+      </c>
       <c r="BI55" s="2"/>
       <c r="BJ55" s="2"/>
       <c r="BK55" s="2"/>
+      <c r="BL55" s="2"/>
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
@@ -7247,7 +7396,7 @@
       <c r="AV56" s="2"/>
       <c r="AW56" s="2"/>
       <c r="AX56" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AY56" s="2"/>
       <c r="AZ56" s="2" t="n">
@@ -7274,29 +7423,30 @@
       <c r="BI56" s="2"/>
       <c r="BJ56" s="2"/>
       <c r="BK56" s="2"/>
+      <c r="BL56" s="2"/>
     </row>
     <row r="57">
       <c r="A57" s="3" t="n">
         <v>1</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D57" s="3"/>
       <c r="E57" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
@@ -7348,7 +7498,7 @@
       <c r="AV57" s="3"/>
       <c r="AW57" s="3"/>
       <c r="AX57" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AY57" s="3"/>
       <c r="AZ57" s="3" t="n">
@@ -7375,6 +7525,7 @@
       <c r="BI57" s="3"/>
       <c r="BJ57" s="3"/>
       <c r="BK57" s="3"/>
+      <c r="BL57" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>